<commit_message>
atualizando tudo para o meu modelo v1
</commit_message>
<xml_diff>
--- a/Penetracao_tecnologias_sucata.xlsx
+++ b/Penetracao_tecnologias_sucata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,6 +50,117 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
   <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>DR-NG</t>
+  </si>
+  <si>
+    <t>DR-H2</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>BF-BOF-CCS</t>
+  </si>
+  <si>
+    <t>RESUMO DOS RESULTADOS</t>
+  </si>
+  <si>
+    <t>Estatística de regressão</t>
+  </si>
+  <si>
+    <t>R múltiplo</t>
+  </si>
+  <si>
+    <t>R-Quadrado</t>
+  </si>
+  <si>
+    <t>R-quadrado ajustado</t>
+  </si>
+  <si>
+    <t>Erro padrão</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>gl</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F de significação</t>
+  </si>
+  <si>
+    <t>Regressão</t>
+  </si>
+  <si>
+    <t>Resíduo</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Coeficientes</t>
+  </si>
+  <si>
+    <t>Stat t</t>
+  </si>
+  <si>
+    <t>valor-P</t>
+  </si>
+  <si>
+    <t>95% inferiores</t>
+  </si>
+  <si>
+    <t>95% superiores</t>
+  </si>
+  <si>
+    <t>Inferior 95.0%</t>
+  </si>
+  <si>
+    <t>Superior 95.0%</t>
+  </si>
+  <si>
+    <t>Interseção</t>
+  </si>
+  <si>
+    <t>Variável X 1</t>
+  </si>
+  <si>
+    <t>Variável X 2</t>
+  </si>
+  <si>
+    <t>Variável X 3</t>
+  </si>
+  <si>
+    <t>Variável X 4</t>
+  </si>
+  <si>
+    <t>Variável X 5</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Y previsto</t>
+  </si>
+  <si>
+    <t>Resíduos</t>
+  </si>
+  <si>
     <t>Mitigation measure</t>
   </si>
   <si>
@@ -171,117 +282,6 @@
   </si>
   <si>
     <t>Recuperacao de gas natural de alto-forno</t>
-  </si>
-  <si>
-    <t>DR-NG</t>
-  </si>
-  <si>
-    <t>DR-H2</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>BF-BOF-CCS</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>RESUMO DOS RESULTADOS</t>
-  </si>
-  <si>
-    <t>Estatística de regressão</t>
-  </si>
-  <si>
-    <t>R múltiplo</t>
-  </si>
-  <si>
-    <t>R-Quadrado</t>
-  </si>
-  <si>
-    <t>R-quadrado ajustado</t>
-  </si>
-  <si>
-    <t>Erro padrão</t>
-  </si>
-  <si>
-    <t>Observações</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Regressão</t>
-  </si>
-  <si>
-    <t>Resíduo</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Interseção</t>
-  </si>
-  <si>
-    <t>gl</t>
-  </si>
-  <si>
-    <t>SQ</t>
-  </si>
-  <si>
-    <t>MQ</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>F de significação</t>
-  </si>
-  <si>
-    <t>Coeficientes</t>
-  </si>
-  <si>
-    <t>Stat t</t>
-  </si>
-  <si>
-    <t>valor-P</t>
-  </si>
-  <si>
-    <t>95% inferiores</t>
-  </si>
-  <si>
-    <t>95% superiores</t>
-  </si>
-  <si>
-    <t>Inferior 95.0%</t>
-  </si>
-  <si>
-    <t>Superior 95.0%</t>
-  </si>
-  <si>
-    <t>Variável X 1</t>
-  </si>
-  <si>
-    <t>Variável X 2</t>
-  </si>
-  <si>
-    <t>Variável X 3</t>
-  </si>
-  <si>
-    <t>Observação</t>
-  </si>
-  <si>
-    <t>Y previsto</t>
-  </si>
-  <si>
-    <t>Resíduos</t>
-  </si>
-  <si>
-    <t>Variável X 4</t>
-  </si>
-  <si>
-    <t>Variável X 5</t>
   </si>
   <si>
     <r>
@@ -345,12 +345,12 @@
     <t>where S is the scrap amount available in year t and n is the share of each steel product group i. Each group has a specific lifetime T and recovery rate ρ. The estimated values for these parameters are presented in Supplementary Material B. Constant γ represents steel losses in obsolete stocks, which were assumed to be 10% over the analyzed period. Finally, P is the total apparent steel consumption (domestic sales plus imports)</t>
   </si>
   <si>
+    <t>Produção anual de aço</t>
+  </si>
+  <si>
     <t>Consumo aparente</t>
   </si>
   <si>
-    <t>Produção anual de aço</t>
-  </si>
-  <si>
     <t>Oferta de sucata</t>
   </si>
   <si>
@@ -369,10 +369,10 @@
     <t xml:space="preserve">(IABr 2018) 2013-2017 </t>
   </si>
   <si>
+    <t>(VASQUES 2009)</t>
+  </si>
+  <si>
     <t>mean values</t>
-  </si>
-  <si>
-    <t>(VASQUES 2009)</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3633,8 +3633,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>150945</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1251766</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3751,7 +3751,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4053,16 +4053,16 @@
       <selection activeCell="B5" sqref="B5:AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -4158,9 +4158,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4256,9 +4256,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4374,9 +4374,9 @@
         <v>0.98566501672383067</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4495,9 +4495,9 @@
         <v>0.98880746303425338</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4593,7 +4593,7 @@
         <v>0.98566501672383067</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32">
       <c r="B10">
         <v>0</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32">
       <c r="B11">
         <v>0.01</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32">
       <c r="B12">
         <f>LN(1/B11-1)</f>
         <v>4.5951198501345898</v>
@@ -4699,140 +4699,140 @@
         <v>-4.5951198501345836</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19">
       <c r="B21" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="N21" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" ht="15" thickBot="1"/>
+    <row r="23" spans="2:19">
       <c r="B23" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>0.99267568197366185</v>
       </c>
       <c r="N24" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O24">
         <v>0.98547585648208091</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>0.98540500958187471</v>
       </c>
       <c r="N25" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="O25">
         <v>0.97116266370909099</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>-1.6666666666666667</v>
       </c>
       <c r="N26" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="O26">
         <v>-1.6666666666666667</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19">
       <c r="B27" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>0.47344404566606335</v>
       </c>
       <c r="N27" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="O27">
         <v>0.66549427366887892</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:19" ht="15" thickBot="1">
       <c r="B28" s="2" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="O28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:19" ht="15" thickBot="1">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="N30" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:19">
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:19">
       <c r="B32" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -4850,7 +4850,7 @@
         <v>#NUM!</v>
       </c>
       <c r="N32" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="O32">
         <v>5</v>
@@ -4868,9 +4868,9 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:22">
       <c r="B33" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -4882,7 +4882,7 @@
         <v>0.22414926437664948</v>
       </c>
       <c r="N33" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="O33">
         <v>3</v>
@@ -4894,9 +4894,9 @@
         <v>0.44288262828606872</v>
       </c>
     </row>
-    <row r="34" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:22" ht="15" thickBot="1">
       <c r="B34" s="2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2">
         <v>8</v>
@@ -4908,7 +4908,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="N34" s="2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="O34" s="2">
         <v>8</v>
@@ -4920,62 +4920,62 @@
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:22" ht="15" thickBot="1"/>
+    <row r="36" spans="2:22">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:22">
       <c r="B37" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="I37">
         <v>4.3193113597126049E+180</v>
@@ -4984,7 +4984,7 @@
         <v>-4.3193113597126049E+180</v>
       </c>
       <c r="N37" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="U37">
         <v>0</v>
@@ -4993,9 +4993,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:22">
       <c r="B38" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="I38">
         <v>4.0648952756419708E+236</v>
@@ -5004,7 +5004,7 @@
         <v>-4.0648952756419708E+236</v>
       </c>
       <c r="N38" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="U38">
         <v>4.9504481611159477E-279</v>
@@ -5013,9 +5013,9 @@
         <v>4.9504481611159477E-279</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:22">
       <c r="B39" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="I39">
         <v>5.2854427649073977E+180</v>
@@ -5024,7 +5024,7 @@
         <v>5.2854427649073977E+180</v>
       </c>
       <c r="N39" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="U39">
         <v>2.6702254141192463E-307</v>
@@ -5033,9 +5033,9 @@
         <v>2.6703321136943701E-307</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:22">
       <c r="B40" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="I40">
         <v>8.4830293728986485E-270</v>
@@ -5044,7 +5044,7 @@
         <v>-1.6254206095129989E-269</v>
       </c>
       <c r="N40" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="U40">
         <v>-3.210832967359935E-241</v>
@@ -5053,9 +5053,9 @@
         <v>-3.210832967359935E-241</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:22">
       <c r="B41" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C41">
         <v>4.2533921278275022</v>
@@ -5082,7 +5082,7 @@
         <v>5.4190009645429935</v>
       </c>
       <c r="N41" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="O41">
         <v>4.2306136245556258</v>
@@ -5109,9 +5109,9 @@
         <v>5.8711317495552517</v>
       </c>
     </row>
-    <row r="42" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:22" ht="15" thickBot="1">
       <c r="B42" s="2" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C42" s="2">
         <v>-0.37976715427031266</v>
@@ -5138,7 +5138,7 @@
         <v>-0.29484668566304501</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="O42" s="2">
         <v>-0.42306136245556247</v>
@@ -5165,19 +5165,19 @@
         <v>-0.28911361845434669</v>
       </c>
     </row>
-    <row r="45" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:22" ht="15" thickBot="1"/>
+    <row r="46" spans="2:22">
       <c r="B46" s="3" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="47" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:22" ht="15" thickBot="1">
       <c r="B47" s="2">
         <v>1</v>
       </c>
@@ -5202,56 +5202,56 @@
       <selection activeCell="L30" sqref="L30:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>0.37</v>
@@ -5266,7 +5266,7 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J2">
         <v>0.185</v>
@@ -5279,18 +5279,18 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>0.12121999999999999</v>
@@ -5305,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J3">
         <v>0.12121999999999999</v>
@@ -5318,18 +5318,18 @@
         <v>0.12121999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E4">
         <v>0.55000000000000004</v>
@@ -5344,7 +5344,7 @@
         <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J4">
         <v>0.27500000000000002</v>
@@ -5357,18 +5357,18 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>0.56999999999999995</v>
@@ -5383,7 +5383,7 @@
         <v>0.25</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="J5">
         <v>0.14249999999999999</v>
@@ -5396,18 +5396,18 @@
         <v>0.14249999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>0.9</v>
@@ -5422,7 +5422,7 @@
         <v>0.25</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <v>0.22500000000000001</v>
@@ -5435,18 +5435,18 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>7.0000000000000007E-2</v>
@@ -5461,7 +5461,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J7">
         <v>7.0000000000000007E-2</v>
@@ -5474,18 +5474,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E8">
         <v>0.92</v>
@@ -5500,7 +5500,7 @@
         <v>0.25</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J8">
         <v>0.23</v>
@@ -5513,18 +5513,18 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>0.55000000000000004</v>
@@ -5539,7 +5539,7 @@
         <v>0.25</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J9">
         <v>0.13750000000000001</v>
@@ -5552,18 +5552,18 @@
         <v>0.13750000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>0.03</v>
@@ -5578,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J10">
         <v>0.03</v>
@@ -5591,18 +5591,18 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>0.3</v>
@@ -5617,7 +5617,7 @@
         <v>0.5</v>
       </c>
       <c r="I11" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J11">
         <v>0.15</v>
@@ -5630,18 +5630,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>0.33</v>
@@ -5656,7 +5656,7 @@
         <v>0.5</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J12">
         <v>0.16500000000000001</v>
@@ -5669,18 +5669,18 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E13">
         <v>0.55000000000000004</v>
@@ -5695,7 +5695,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J13">
         <v>0.27500000000000002</v>
@@ -5708,18 +5708,18 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>0.09</v>
@@ -5734,7 +5734,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J14">
         <v>0.09</v>
@@ -5747,18 +5747,18 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E15">
         <v>0.09</v>
@@ -5773,7 +5773,7 @@
         <v>0.75</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J15">
         <v>6.7500000000000004E-2</v>
@@ -5786,18 +5786,18 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <v>0.56999999999999995</v>
@@ -5812,7 +5812,7 @@
         <v>0.25</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J16">
         <v>0.14249999999999999</v>
@@ -5825,18 +5825,18 @@
         <v>0.14249999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <v>0.9</v>
@@ -5851,7 +5851,7 @@
         <v>0.25</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J17">
         <v>0.22500000000000001</v>
@@ -5864,18 +5864,18 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E18">
         <v>7.0000000000000007E-2</v>
@@ -5890,7 +5890,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J18">
         <v>7.0000000000000007E-2</v>
@@ -5903,18 +5903,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E19">
         <v>0.55000000000000004</v>
@@ -5929,7 +5929,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J19">
         <v>4.1250000000000002E-2</v>
@@ -5942,18 +5942,18 @@
         <v>4.1250000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E20">
         <v>0.55000000000000004</v>
@@ -5968,7 +5968,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J20">
         <v>4.1250000000000002E-2</v>
@@ -5981,18 +5981,18 @@
         <v>4.1250000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E21">
         <v>0.03</v>
@@ -6007,7 +6007,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J21">
         <v>0.03</v>
@@ -6020,18 +6020,18 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E22">
         <v>0.3</v>
@@ -6046,7 +6046,7 @@
         <v>0.5</v>
       </c>
       <c r="I22" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J22">
         <v>0.15</v>
@@ -6059,18 +6059,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E23">
         <v>0.33</v>
@@ -6085,7 +6085,7 @@
         <v>0.5</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J23">
         <v>0.16500000000000001</v>
@@ -6098,18 +6098,18 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E24">
         <v>7.0000000000000007E-2</v>
@@ -6124,7 +6124,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J24">
         <v>7.0000000000000007E-2</v>
@@ -6137,18 +6137,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E25">
         <v>0.14000000000000001</v>
@@ -6163,7 +6163,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J25">
         <v>0.14000000000000001</v>
@@ -6176,18 +6176,18 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E26">
         <v>0.11</v>
@@ -6202,7 +6202,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J26">
         <v>0.11</v>
@@ -6215,18 +6215,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E27">
         <v>0.13</v>
@@ -6241,7 +6241,7 @@
         <v>0.5</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J27">
         <v>6.5000000000000002E-2</v>
@@ -6254,18 +6254,18 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E28">
         <v>0.7</v>
@@ -6280,7 +6280,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J28">
         <v>0.7</v>
@@ -6293,18 +6293,18 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E29">
         <v>0.21</v>
@@ -6319,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J29">
         <v>0.21</v>
@@ -6332,18 +6332,18 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E30">
         <v>0.55000000000000004</v>
@@ -6358,7 +6358,7 @@
         <v>0.5</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J30">
         <v>0.27500000000000002</v>
@@ -6371,18 +6371,18 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E31">
         <v>0.09</v>
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J31">
         <v>0.09</v>
@@ -6410,18 +6410,18 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E32">
         <v>0.09</v>
@@ -6436,7 +6436,7 @@
         <v>0.75</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J32">
         <v>6.7500000000000004E-2</v>
@@ -6449,18 +6449,18 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E33">
         <v>0.56999999999999995</v>
@@ -6475,7 +6475,7 @@
         <v>0.25</v>
       </c>
       <c r="I33" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J33">
         <v>0.14249999999999999</v>
@@ -6488,18 +6488,18 @@
         <v>0.14249999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E34">
         <v>0.9</v>
@@ -6514,7 +6514,7 @@
         <v>0.25</v>
       </c>
       <c r="I34" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J34">
         <v>0.22500000000000001</v>
@@ -6527,18 +6527,18 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E35">
         <v>7.0000000000000007E-2</v>
@@ -6553,7 +6553,7 @@
         <v>0.5</v>
       </c>
       <c r="I35" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J35">
         <v>3.5000000000000003E-2</v>
@@ -6580,17 +6580,17 @@
       <selection activeCell="B27" sqref="B27:AF27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="61.5546875" customWidth="1"/>
+    <col min="1" max="1" width="61.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="35" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="47" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="47" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:82" ht="15" thickBot="1">
       <c r="A1" s="26" t="s">
         <v>78</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:82">
       <c r="A2" s="27"/>
       <c r="B2" s="7" t="s">
         <v>82</v>
@@ -6706,7 +6706,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:82">
       <c r="A3" s="8" t="s">
         <v>84</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:82">
       <c r="A4" s="11" t="s">
         <v>85</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>1.2222222222222223</v>
       </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:82">
       <c r="A5" s="8" t="s">
         <v>86</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>1.142857142857143</v>
       </c>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:82">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:82" ht="15" thickBot="1">
       <c r="A7" s="14" t="s">
         <v>88</v>
       </c>
@@ -7402,12 +7402,12 @@
         <v>1.4999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:82" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:82" ht="86.45">
       <c r="A9" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:82">
       <c r="B12">
         <v>1970</v>
       </c>
@@ -7652,9 +7652,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:82">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13">
         <v>5000</v>
@@ -7900,9 +7900,9 @@
         <v>64072</v>
       </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:82">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B14">
         <v>5000</v>
@@ -8191,10 +8191,10 @@
         <v>42287.520000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:82">
       <c r="AZ15" s="16"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32">
       <c r="A18" s="8" t="s">
         <v>84</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>3691.7004960000004</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32">
       <c r="A19" s="11" t="s">
         <v>85</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>3291.6076974000007</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32">
       <c r="A20" s="8" t="s">
         <v>86</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>5220.9017942399923</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32">
       <c r="A21" s="11" t="s">
         <v>87</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>2911.4957520000003</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" ht="15" thickBot="1">
       <c r="A22" s="14" t="s">
         <v>88</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32">
       <c r="A23" s="11" t="s">
         <v>93</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>17059.705739639994</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32">
       <c r="A24" s="23">
         <f>B24/B23</f>
         <v>0.96876313670665348</v>
@@ -9075,7 +9075,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32">
       <c r="B26" s="16">
         <f>AZ13*0.24*0.85</f>
         <v>6951.229527272717</v>
@@ -9201,7 +9201,7 @@
         <v>13070.687999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -9234,8 +9234,8 @@
       <c r="AE27" s="17"/>
       <c r="AF27" s="17"/>
     </row>
-    <row r="28" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:32" ht="15" thickBot="1"/>
+    <row r="29" spans="1:32" ht="15" thickBot="1">
       <c r="A29" s="26" t="s">
         <v>78</v>
       </c>
@@ -9249,7 +9249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32">
       <c r="A30" s="27"/>
       <c r="B30" s="7" t="s">
         <v>82</v>
@@ -9279,7 +9279,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32">
       <c r="A31" s="8" t="s">
         <v>84</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32">
       <c r="A32" s="11" t="s">
         <v>85</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>0.95569620253164556</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33" s="8" t="s">
         <v>86</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>7495</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="11" t="s">
         <v>87</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="8" t="s">
         <v>88</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>1.1282051282051282</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36" s="28" t="s">
         <v>95</v>
       </c>
@@ -9421,17 +9421,17 @@
         <v>97</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G36">
         <v>7550</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="15" thickBot="1">
       <c r="A37" s="29"/>
       <c r="B37" s="31"/>
       <c r="C37" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D37" s="31"/>
     </row>

</xml_diff>